<commit_message>
Add "Model Group" column to daily IC reference file for commercial buildings
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_towns_com_bldg_detail.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_towns_com_bldg_detail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\ic_reference_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2AEAA9-C552-4F45-BB8E-99ABF732C558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9BB216-128B-47D0-BB40-F9D40FE0CCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>PARDAT</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Township</t>
+  </si>
+  <si>
+    <t>Model Group</t>
   </si>
 </sst>
 </file>
@@ -581,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK2"/>
+  <dimension ref="A1:BL2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,10 +778,13 @@
         <v>1</v>
       </c>
       <c r="BK1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -966,6 +972,9 @@
         <v>63</v>
       </c>
       <c r="BK2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add "Model Group" column to daily IC reference file for commercial buildings (#782)
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_towns_com_bldg_detail.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_towns_com_bldg_detail.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\ic_reference_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2AEAA9-C552-4F45-BB8E-99ABF732C558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9BB216-128B-47D0-BB40-F9D40FE0CCE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>PARDAT</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Township</t>
+  </si>
+  <si>
+    <t>Model Group</t>
   </si>
 </sst>
 </file>
@@ -581,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BK2"/>
+  <dimension ref="A1:BL2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,10 +778,13 @@
         <v>1</v>
       </c>
       <c r="BK1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -966,6 +972,9 @@
         <v>63</v>
       </c>
       <c r="BK2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BL2" s="1" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>